<commit_message>
arrange the code of scene #86
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Npc.xlsx
+++ b/ConfigData/Xlsx/Npc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Npc" sheetId="1" r:id="rId1"/>
@@ -598,12 +598,6 @@
     <t>Lv</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Func</t>
   </si>
   <si>
@@ -721,6 +715,14 @@
   </si>
   <si>
     <t>0:-1|[Shp44010006]交易|-1|取消</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1409,20 +1411,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K53" totalsRowShown="0">
-  <autoFilter ref="A1:K53">
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter val="*Shp*"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K53"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="MapId"/>
     <tableColumn id="4" name="Lv"/>
-    <tableColumn id="5" name="X"/>
-    <tableColumn id="6" name="Y"/>
+    <tableColumn id="5" name="X1"/>
+    <tableColumn id="6" name="Y1"/>
     <tableColumn id="7" name="Func"/>
     <tableColumn id="8" name="Say"/>
     <tableColumn id="9" name="Answer"/>
@@ -1723,19 +1719,19 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
-    <col min="4" max="7" width="5.75" customWidth="1"/>
-    <col min="8" max="8" width="31.75" customWidth="1"/>
-    <col min="9" max="9" width="64.25" customWidth="1"/>
-    <col min="13" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="7" width="5.77734375" customWidth="1"/>
+    <col min="8" max="8" width="31.77734375" customWidth="1"/>
+    <col min="9" max="9" width="64.21875" customWidth="1"/>
+    <col min="13" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>184</v>
       </c>
@@ -1749,28 +1745,28 @@
         <v>187</v>
       </c>
       <c r="E1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" t="s">
         <v>188</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>189</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J1" t="s">
         <v>190</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>191</v>
       </c>
-      <c r="I1" t="s">
-        <v>194</v>
-      </c>
-      <c r="J1" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -1805,7 +1801,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>173</v>
       </c>
@@ -1840,7 +1836,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>41000001</v>
       </c>
@@ -1872,7 +1868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>41000002</v>
       </c>
@@ -1898,13 +1894,13 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>41000003</v>
       </c>
@@ -1930,7 +1926,7 @@
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J6" t="s">
         <v>9</v>
@@ -1939,7 +1935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>41000004</v>
       </c>
@@ -1971,7 +1967,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>41000005</v>
       </c>
@@ -1997,7 +1993,7 @@
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J8" t="s">
         <v>17</v>
@@ -2006,7 +2002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>41000051</v>
       </c>
@@ -2032,7 +2028,7 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J9" t="s">
         <v>20</v>
@@ -2041,7 +2037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>41000052</v>
       </c>
@@ -2076,7 +2072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>41000053</v>
       </c>
@@ -2111,7 +2107,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>41010003</v>
       </c>
@@ -2143,7 +2139,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>41010004</v>
       </c>
@@ -2169,13 +2165,13 @@
         <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>41010005</v>
       </c>
@@ -2201,13 +2197,13 @@
         <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>41010006</v>
       </c>
@@ -2239,7 +2235,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>41010007</v>
       </c>
@@ -2265,13 +2261,13 @@
         <v>46</v>
       </c>
       <c r="I16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>41010008</v>
       </c>
@@ -2297,13 +2293,13 @@
         <v>49</v>
       </c>
       <c r="I17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>41010009</v>
       </c>
@@ -2329,13 +2325,13 @@
         <v>52</v>
       </c>
       <c r="I18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>41010010</v>
       </c>
@@ -2367,7 +2363,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>41010011</v>
       </c>
@@ -2399,7 +2395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>41010013</v>
       </c>
@@ -2425,13 +2421,13 @@
         <v>62</v>
       </c>
       <c r="I21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>41010014</v>
       </c>
@@ -2463,7 +2459,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>41010015</v>
       </c>
@@ -2489,13 +2485,13 @@
         <v>69</v>
       </c>
       <c r="I23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>41010016</v>
       </c>
@@ -2521,13 +2517,13 @@
         <v>72</v>
       </c>
       <c r="I24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>41010017</v>
       </c>
@@ -2559,7 +2555,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>41010018</v>
       </c>
@@ -2591,7 +2587,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>41010019</v>
       </c>
@@ -2617,13 +2613,13 @@
         <v>83</v>
       </c>
       <c r="I27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J27" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>41010020</v>
       </c>
@@ -2649,13 +2645,13 @@
         <v>86</v>
       </c>
       <c r="I28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>41010021</v>
       </c>
@@ -2681,13 +2677,13 @@
         <v>89</v>
       </c>
       <c r="I29" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>41010022</v>
       </c>
@@ -2719,7 +2715,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>41010023</v>
       </c>
@@ -2751,7 +2747,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>41010024</v>
       </c>
@@ -2783,7 +2779,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>41010025</v>
       </c>
@@ -2815,7 +2811,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>41010026</v>
       </c>
@@ -2847,7 +2843,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>41010027</v>
       </c>
@@ -2873,13 +2869,13 @@
         <v>111</v>
       </c>
       <c r="I35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>41010028</v>
       </c>
@@ -2905,13 +2901,13 @@
         <v>114</v>
       </c>
       <c r="I36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J36" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>41010029</v>
       </c>
@@ -2943,7 +2939,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>41010030</v>
       </c>
@@ -2975,7 +2971,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>41010031</v>
       </c>
@@ -3007,7 +3003,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>41010050</v>
       </c>
@@ -3039,7 +3035,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41012002</v>
       </c>
@@ -3065,13 +3061,13 @@
         <v>133</v>
       </c>
       <c r="I41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J41" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41012003</v>
       </c>
@@ -3097,13 +3093,13 @@
         <v>136</v>
       </c>
       <c r="I42" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J42" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41012004</v>
       </c>
@@ -3129,13 +3125,13 @@
         <v>139</v>
       </c>
       <c r="I43" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J43" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41012005</v>
       </c>
@@ -3161,13 +3157,13 @@
         <v>142</v>
       </c>
       <c r="I44" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J44" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>41012006</v>
       </c>
@@ -3193,13 +3189,13 @@
         <v>144</v>
       </c>
       <c r="I45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J45" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>41013002</v>
       </c>
@@ -3231,7 +3227,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>41013003</v>
       </c>
@@ -3263,7 +3259,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>41013004</v>
       </c>
@@ -3295,7 +3291,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>41013005</v>
       </c>
@@ -3327,7 +3323,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>41014001</v>
       </c>
@@ -3353,13 +3349,13 @@
         <v>160</v>
       </c>
       <c r="I50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J50" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>41014002</v>
       </c>
@@ -3385,13 +3381,13 @@
         <v>163</v>
       </c>
       <c r="I51" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J51" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>41014003</v>
       </c>
@@ -3417,13 +3413,13 @@
         <v>166</v>
       </c>
       <c r="I52" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J52" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>41014004</v>
       </c>
@@ -3449,7 +3445,7 @@
         <v>169</v>
       </c>
       <c r="I53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J53" t="s">
         <v>170</v>

</xml_diff>